<commit_message>
Added Tabbar and Toolbar tests to DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Tabbar_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Tabbar_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -424,6 +424,110 @@
 wait(5);
 TakeNativeScreenshot(VT200_0578);
 validate6;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Native Tabbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0576
+};
+validate4
+{
+validate_Screenshot=VT200_0576_new
+};
+validate5
+{
+validate_Text_Exists=VT200-0596
+};
+validate6
+{
+validate_Screenshot=VT200_0596
+};</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(tabbar_test_link);
+validate2;
+SelectTestToRun(VT200_0576_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+TakeScreenshot(VT200_0576_new);
+validate4;
+SwitchApp(NATIVE_APP);
+wait(2);
+link_Click(VT200_0576_mainpage_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+SelectTestToRun(VT200_0596_string);
+ClickRunTest(runtest_top_xpath);
+validate5;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+TakeNativeScreenshot(VT200_0596);
+validate6;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(5);
+validate1;
+link_Click(tabbar_test_link);
+validate2;
+SelectTestToRun(VT200_0576_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+TakeScreenshot(VT200_0576_new);
+validate4;
+SwitchApp(NATIVE_APP);
+wait(2);
+link_Click(VT200_0576_mainpage_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+SelectTestToRun(VT200_0595_string);
+ClickRunTest(runtest_top_xpath);
+validate5;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+TakeNativeScreenshot(VT200_0595);
+validate6;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Native Tabbar JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0576
+};
+validate4
+{
+validate_Screenshot=VT200_0576_new
+};
+validate5
+{
+validate_Text_Exists=VT200-0595
+};
+validate6
+{
+validate_Screenshot=VT200_0595
+};
+</t>
   </si>
 </sst>
 </file>
@@ -460,7 +564,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -511,11 +615,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -525,6 +640,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -831,7 +949,7 @@
     <col min="1" max="1" width="11.140625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.5703125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="37.140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -981,7 +1099,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="79.5" thickBot="1">
+    <row r="6" spans="1:11" ht="282" thickBot="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -989,20 +1107,26 @@
         <v>1</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="102" thickBot="1">
+    <row r="7" spans="1:11" ht="270.75" thickBot="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1010,15 +1134,21 @@
         <v>1</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1184,6 +1314,9 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="D14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>